<commit_message>
Taxonomiecodes voor SCRUM vaardigheden toegevoegd
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eb0095856\Projecten\Leerlijn-Content-SE-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B9D039-4F04-4A6F-A498-5C853ACBEAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DDF457-4D4B-4536-83CC-D00885F13F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7013DF88-B919-4E44-A3B6-EFF7F9C231E9}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{7013DF88-B919-4E44-A3B6-EFF7F9C231E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="314">
   <si>
     <t>TC-1</t>
   </si>
@@ -906,6 +906,81 @@
   </si>
   <si>
     <t>Vaststellen-doelen</t>
+  </si>
+  <si>
+    <t>Bepalen-werklast</t>
+  </si>
+  <si>
+    <t>In-kaart-brengen-afhankelijkheden</t>
+  </si>
+  <si>
+    <t>Kiezen-user-stories</t>
+  </si>
+  <si>
+    <t>Toevoegen taken aan user story</t>
+  </si>
+  <si>
+    <t>Opstellen-product-backlog</t>
+  </si>
+  <si>
+    <t>Prioriteren-product-backlog</t>
+  </si>
+  <si>
+    <t>Toevoegen-acceptatiecriteria</t>
+  </si>
+  <si>
+    <t>Monitoren-voortgang-sprintdoel</t>
+  </si>
+  <si>
+    <t>Uiten-belemmeringen</t>
+  </si>
+  <si>
+    <t>Inzichtelijk-maken-voortgang</t>
+  </si>
+  <si>
+    <t>Oplossen-belemmeringen</t>
+  </si>
+  <si>
+    <t>Ondersteunen-teamlid</t>
+  </si>
+  <si>
+    <t>Peerreviewen-werk</t>
+  </si>
+  <si>
+    <t>Werk-presenteren</t>
+  </si>
+  <si>
+    <t>Ophalen-feedback</t>
+  </si>
+  <si>
+    <t>Feedback-verwerken</t>
+  </si>
+  <si>
+    <t>Kiezen-werkvorm</t>
+  </si>
+  <si>
+    <t>Feedback-geven</t>
+  </si>
+  <si>
+    <t>Feedback-ontvangen</t>
+  </si>
+  <si>
+    <t>Noteren-actiepunten</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Aangeven-behoeften</t>
+  </si>
+  <si>
+    <t>Aangeven-grenzen</t>
+  </si>
+  <si>
+    <t>Afstemmen-op-behoeften-omgeving</t>
+  </si>
+  <si>
+    <t>Opstellen-productafspraken</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1423,11 +1498,16 @@
     <xf numFmtId="0" fontId="9" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="76">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1625,6 +1705,146 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2666,61 +2886,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}" name="Tabel3" displayName="Tabel3" ref="A1:P155" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58">
-  <autoFilter ref="A1:P155" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}" name="Tabel3" displayName="Tabel3" ref="A1:P176" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72">
+  <autoFilter ref="A1:P176" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}"/>
   <tableColumns count="16">
-    <tableColumn id="2" xr3:uid="{F8A50546-3BB2-41F8-99A7-821FFAEA9EA0}" name="TC-1" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{41734F87-6DB1-4AC3-80CE-250B23378554}" name="TC-2" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{5B30DF97-0362-47CA-9FEB-983BDA2DF844}" name="Proces" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{DDC7FBE8-1A18-4596-8FBD-1F40B9F94AA0}" name="Processtap" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{15170496-2005-43A7-AD43-CFD4F0B25656}" name="Onderwerp" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{AD473AEC-8FAD-46C0-A48A-A65E296DBE11}" name="PS" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{1591AA9A-3ED6-44E5-A48A-E9910C5A2DDC}" name="LT" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{343866B0-4820-4E45-9596-524C0A3E0DB4}" name="OI" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{B3D04D72-920A-4859-8170-8854154E6BEE}" name="PI" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{DAE26EF7-02E2-4493-9827-F044C9947102}" name="DT" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{66861921-DC42-4E48-9995-22D71902D0E6}" name="Auteur" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{F8A50546-3BB2-41F8-99A7-821FFAEA9EA0}" name="TC-1" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{41734F87-6DB1-4AC3-80CE-250B23378554}" name="TC-2" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{5B30DF97-0362-47CA-9FEB-983BDA2DF844}" name="Proces" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{DDC7FBE8-1A18-4596-8FBD-1F40B9F94AA0}" name="Processtap" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{15170496-2005-43A7-AD43-CFD4F0B25656}" name="Onderwerp" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{AD473AEC-8FAD-46C0-A48A-A65E296DBE11}" name="PS" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{1591AA9A-3ED6-44E5-A48A-E9910C5A2DDC}" name="LT" dataDxfId="65"/>
+    <tableColumn id="9" xr3:uid="{343866B0-4820-4E45-9596-524C0A3E0DB4}" name="OI" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{B3D04D72-920A-4859-8170-8854154E6BEE}" name="PI" dataDxfId="63"/>
+    <tableColumn id="11" xr3:uid="{DAE26EF7-02E2-4493-9827-F044C9947102}" name="DT" dataDxfId="62"/>
+    <tableColumn id="12" xr3:uid="{66861921-DC42-4E48-9995-22D71902D0E6}" name="Auteur" dataDxfId="61"/>
     <tableColumn id="13" xr3:uid="{41E829DC-30B4-4ED6-A23E-6E86A90CC847}" name="Status"/>
-    <tableColumn id="14" xr3:uid="{4DEA7C20-4CDB-4765-A2ED-2DAE0C74EA88}" name="Les" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{BA1A1DC9-E1C8-41C8-8B22-98655139BA61}" name="Week" dataDxfId="45"/>
-    <tableColumn id="16" xr3:uid="{FEFBF060-7975-4841-BB25-4FD9EA20FCE9}" name="Vak" dataDxfId="44"/>
-    <tableColumn id="17" xr3:uid="{DC49865F-5E2A-4A41-9018-4460A5231335}" name="Opmerking" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{4DEA7C20-4CDB-4765-A2ED-2DAE0C74EA88}" name="Les" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{BA1A1DC9-E1C8-41C8-8B22-98655139BA61}" name="Week" dataDxfId="59"/>
+    <tableColumn id="16" xr3:uid="{FEFBF060-7975-4841-BB25-4FD9EA20FCE9}" name="Vak" dataDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{DC49865F-5E2A-4A41-9018-4460A5231335}" name="Opmerking" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}" name="Tabel46" displayName="Tabel46" ref="A1:M25" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}" name="Tabel46" displayName="Tabel46" ref="A1:M25" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A1:M25" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}"/>
   <tableColumns count="13">
-    <tableColumn id="2" xr3:uid="{1535D98C-E0EE-4D42-BCEB-E5B9CE3EB61D}" name="TC-1" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{626D3CCE-98FA-446A-9492-EFF5B77FBEE7}" name="TC-2" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{7D9467F0-D231-479A-AC4D-EFCFCDA0F355}" name="Proces" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{563F1A23-B95F-4820-8982-FD4C397E7132}" name="Processtap" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{6EB4EFB7-2E6E-49E8-8B36-E5A953066F34}" name="Onderwerp" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{952C00F6-C03B-46BB-8BDD-48716B660A03}" name="PS" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{905E3EDF-F38D-471C-BAF6-5E4C96FF3FB2}" name="LT" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{8DFE5EC7-2595-4617-8FC0-FDDA89438F44}" name="OI" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{557B5D16-5B65-4AF7-BD7B-FB0218A7C1B3}" name="PI" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{9F6BDCD6-BD58-4752-B392-4BDB07F65BF9}" name="DT" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{265C90D0-C2F9-46F3-BC15-46853C80AE44}" name="Auteur" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{56238B06-B929-4176-9193-3DBF61BD24F4}" name="Reviewer" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{5A7CC1D3-6CDF-46C8-BAD6-5021F68425FC}" name="Status" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{1535D98C-E0EE-4D42-BCEB-E5B9CE3EB61D}" name="TC-1" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{626D3CCE-98FA-446A-9492-EFF5B77FBEE7}" name="TC-2" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{7D9467F0-D231-479A-AC4D-EFCFCDA0F355}" name="Proces" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{563F1A23-B95F-4820-8982-FD4C397E7132}" name="Processtap" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{6EB4EFB7-2E6E-49E8-8B36-E5A953066F34}" name="Onderwerp" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{952C00F6-C03B-46BB-8BDD-48716B660A03}" name="PS" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{905E3EDF-F38D-471C-BAF6-5E4C96FF3FB2}" name="LT" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{8DFE5EC7-2595-4617-8FC0-FDDA89438F44}" name="OI" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{557B5D16-5B65-4AF7-BD7B-FB0218A7C1B3}" name="PI" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{9F6BDCD6-BD58-4752-B392-4BDB07F65BF9}" name="DT" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{265C90D0-C2F9-46F3-BC15-46853C80AE44}" name="Auteur" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{56238B06-B929-4176-9193-3DBF61BD24F4}" name="Reviewer" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{5A7CC1D3-6CDF-46C8-BAD6-5021F68425FC}" name="Status" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}" name="Tabel2" displayName="Tabel2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}" name="Tabel2" displayName="Tabel2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:E29" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E0D87A47-D7F7-498A-A22E-05A996992FE5}" name="Id" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{A3888C5B-B532-4621-A573-477CB568DA88}" name="SSDLC" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{E1227983-22D3-4B85-9382-7BE0428CF806}" name="Proces" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{25EAD8F8-D89A-4F34-8AE3-23D6D7363D47}" name="Processtap" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{DCD8D2DD-F7D1-48E7-8B06-F484930BAD1C}" name="Taxonomiecode-deel-1" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{E0D87A47-D7F7-498A-A22E-05A996992FE5}" name="Id" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{A3888C5B-B532-4621-A573-477CB568DA88}" name="SSDLC" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{E1227983-22D3-4B85-9382-7BE0428CF806}" name="Proces" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{25EAD8F8-D89A-4F34-8AE3-23D6D7363D47}" name="Processtap" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{DCD8D2DD-F7D1-48E7-8B06-F484930BAD1C}" name="Taxonomiecode-deel-1" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3043,24 +3263,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C8AE46-0301-40E0-97E1-E2E70FD5D32D}">
-  <dimension ref="A1:P155"/>
+  <dimension ref="A1:P181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA137" sqref="AA137"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -3110,7 +3330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
@@ -3152,7 +3372,7 @@
       <c r="O2" s="31"/>
       <c r="P2" s="45"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>16</v>
       </c>
@@ -3192,7 +3412,7 @@
       <c r="O3" s="31"/>
       <c r="P3" s="45"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>16</v>
       </c>
@@ -3232,7 +3452,7 @@
       <c r="O4" s="31"/>
       <c r="P4" s="45"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>16</v>
       </c>
@@ -3272,7 +3492,7 @@
       <c r="O5" s="31"/>
       <c r="P5" s="45"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>16</v>
       </c>
@@ -3312,7 +3532,7 @@
       <c r="O6" s="31"/>
       <c r="P6" s="45"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>16</v>
       </c>
@@ -3352,7 +3572,7 @@
       <c r="O7" s="31"/>
       <c r="P7" s="45"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>16</v>
       </c>
@@ -3392,7 +3612,7 @@
       <c r="O8" s="31"/>
       <c r="P8" s="45"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
@@ -3432,7 +3652,7 @@
       <c r="O9" s="31"/>
       <c r="P9" s="45"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>16</v>
       </c>
@@ -3472,7 +3692,7 @@
       <c r="O10" s="31"/>
       <c r="P10" s="45"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>16</v>
       </c>
@@ -3512,7 +3732,7 @@
       <c r="O11" s="31"/>
       <c r="P11" s="45"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
@@ -3552,7 +3772,7 @@
       <c r="O12" s="31"/>
       <c r="P12" s="45"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>16</v>
       </c>
@@ -3592,7 +3812,7 @@
       <c r="O13" s="31"/>
       <c r="P13" s="45"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>36</v>
       </c>
@@ -3632,7 +3852,7 @@
       <c r="O14" s="31"/>
       <c r="P14" s="45"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
@@ -3672,7 +3892,7 @@
       <c r="O15" s="31"/>
       <c r="P15" s="45"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>36</v>
       </c>
@@ -3712,7 +3932,7 @@
       <c r="O16" s="31"/>
       <c r="P16" s="45"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>41</v>
       </c>
@@ -3752,7 +3972,7 @@
       <c r="O17" s="31"/>
       <c r="P17" s="45"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
         <v>41</v>
       </c>
@@ -3792,7 +4012,7 @@
       <c r="O18" s="31"/>
       <c r="P18" s="45"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>41</v>
       </c>
@@ -3832,7 +4052,7 @@
       <c r="O19" s="31"/>
       <c r="P19" s="45"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
@@ -3872,7 +4092,7 @@
       <c r="O20" s="31"/>
       <c r="P20" s="45"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>41</v>
       </c>
@@ -3912,7 +4132,7 @@
       <c r="O21" s="31"/>
       <c r="P21" s="45"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>41</v>
       </c>
@@ -3952,7 +4172,7 @@
       <c r="O22" s="31"/>
       <c r="P22" s="45"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>41</v>
       </c>
@@ -3992,7 +4212,7 @@
       <c r="O23" s="31"/>
       <c r="P23" s="45"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>41</v>
       </c>
@@ -4032,7 +4252,7 @@
       <c r="O24" s="31"/>
       <c r="P24" s="45"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>41</v>
       </c>
@@ -4072,7 +4292,7 @@
       <c r="O25" s="31"/>
       <c r="P25" s="45"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>41</v>
       </c>
@@ -4112,7 +4332,7 @@
       <c r="O26" s="31"/>
       <c r="P26" s="45"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>41</v>
       </c>
@@ -4152,7 +4372,7 @@
       <c r="O27" s="31"/>
       <c r="P27" s="45"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>41</v>
       </c>
@@ -4192,7 +4412,7 @@
       <c r="O28" s="31"/>
       <c r="P28" s="45"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>41</v>
       </c>
@@ -4232,7 +4452,7 @@
       <c r="O29" s="31"/>
       <c r="P29" s="45"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>41</v>
       </c>
@@ -4272,7 +4492,7 @@
       <c r="O30" s="31"/>
       <c r="P30" s="45"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>41</v>
       </c>
@@ -4322,7 +4542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>41</v>
       </c>
@@ -4362,7 +4582,7 @@
       <c r="O32" s="31"/>
       <c r="P32" s="45"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>68</v>
       </c>
@@ -4400,7 +4620,7 @@
       <c r="O33" s="31"/>
       <c r="P33" s="45"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>68</v>
       </c>
@@ -4438,7 +4658,7 @@
       <c r="O34" s="31"/>
       <c r="P34" s="45"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>73</v>
       </c>
@@ -4478,7 +4698,7 @@
       <c r="O35" s="31"/>
       <c r="P35" s="45"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>76</v>
       </c>
@@ -4516,7 +4736,7 @@
       <c r="O36" s="31"/>
       <c r="P36" s="45"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>80</v>
       </c>
@@ -4556,7 +4776,7 @@
       <c r="O37" s="31"/>
       <c r="P37" s="45"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>68</v>
       </c>
@@ -4596,7 +4816,7 @@
       <c r="O38" s="31"/>
       <c r="P38" s="45"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>85</v>
       </c>
@@ -4634,7 +4854,7 @@
       <c r="O39" s="31"/>
       <c r="P39" s="45"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>89</v>
       </c>
@@ -4674,7 +4894,7 @@
       <c r="O40" s="31"/>
       <c r="P40" s="45"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>93</v>
       </c>
@@ -4714,7 +4934,7 @@
       <c r="O41" s="31"/>
       <c r="P41" s="45"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>68</v>
       </c>
@@ -4754,7 +4974,7 @@
       <c r="O42" s="31"/>
       <c r="P42" s="45"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>97</v>
       </c>
@@ -4794,7 +5014,7 @@
       <c r="O43" s="31"/>
       <c r="P43" s="45"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>101</v>
       </c>
@@ -4834,7 +5054,7 @@
       <c r="O44" s="31"/>
       <c r="P44" s="45"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>41</v>
       </c>
@@ -4874,7 +5094,7 @@
       <c r="O45" s="31"/>
       <c r="P45" s="45"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
         <v>97</v>
       </c>
@@ -4914,7 +5134,7 @@
       <c r="O46" s="31"/>
       <c r="P46" s="45"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
         <v>97</v>
       </c>
@@ -4954,7 +5174,7 @@
       <c r="O47" s="31"/>
       <c r="P47" s="45"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>97</v>
       </c>
@@ -4994,7 +5214,7 @@
       <c r="O48" s="31"/>
       <c r="P48" s="45"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
         <v>97</v>
       </c>
@@ -5034,7 +5254,7 @@
       <c r="O49" s="31"/>
       <c r="P49" s="45"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
         <v>97</v>
       </c>
@@ -5074,7 +5294,7 @@
       <c r="O50" s="31"/>
       <c r="P50" s="45"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
         <v>97</v>
       </c>
@@ -5114,7 +5334,7 @@
       <c r="O51" s="31"/>
       <c r="P51" s="45"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
         <v>97</v>
       </c>
@@ -5154,7 +5374,7 @@
       <c r="O52" s="31"/>
       <c r="P52" s="45"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>97</v>
       </c>
@@ -5194,7 +5414,7 @@
       <c r="O53" s="31"/>
       <c r="P53" s="45"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
         <v>97</v>
       </c>
@@ -5234,7 +5454,7 @@
       <c r="O54" s="31"/>
       <c r="P54" s="45"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
         <v>97</v>
       </c>
@@ -5274,7 +5494,7 @@
       <c r="O55" s="31"/>
       <c r="P55" s="45"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
         <v>76</v>
       </c>
@@ -5312,7 +5532,7 @@
       <c r="O56" s="31"/>
       <c r="P56" s="45"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
         <v>85</v>
       </c>
@@ -5350,7 +5570,7 @@
       <c r="O57" s="31"/>
       <c r="P57" s="45"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
         <v>85</v>
       </c>
@@ -5388,7 +5608,7 @@
       <c r="O58" s="31"/>
       <c r="P58" s="45"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
         <v>68</v>
       </c>
@@ -5428,7 +5648,7 @@
       <c r="O59" s="31"/>
       <c r="P59" s="45"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="31" t="s">
         <v>41</v>
       </c>
@@ -5468,7 +5688,7 @@
       </c>
       <c r="P60" s="45"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>41</v>
       </c>
@@ -5508,7 +5728,7 @@
       </c>
       <c r="P61" s="45"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
         <v>41</v>
       </c>
@@ -5550,7 +5770,7 @@
       </c>
       <c r="P62" s="45"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="31" t="s">
         <v>41</v>
       </c>
@@ -5596,7 +5816,7 @@
       </c>
       <c r="P63" s="45"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
         <v>41</v>
       </c>
@@ -5642,7 +5862,7 @@
       </c>
       <c r="P64" s="45"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
         <v>41</v>
       </c>
@@ -5688,7 +5908,7 @@
       </c>
       <c r="P65" s="45"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
         <v>41</v>
       </c>
@@ -5734,7 +5954,7 @@
       </c>
       <c r="P66" s="45"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="31" t="s">
         <v>41</v>
       </c>
@@ -5780,7 +6000,7 @@
       </c>
       <c r="P67" s="45"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="31" t="s">
         <v>41</v>
       </c>
@@ -5826,7 +6046,7 @@
       </c>
       <c r="P68" s="45"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="31" t="s">
         <v>41</v>
       </c>
@@ -5872,7 +6092,7 @@
       </c>
       <c r="P69" s="45"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="31" t="s">
         <v>41</v>
       </c>
@@ -5918,7 +6138,7 @@
       </c>
       <c r="P70" s="45"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
         <v>41</v>
       </c>
@@ -5964,7 +6184,7 @@
       </c>
       <c r="P71" s="45"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="31" t="s">
         <v>41</v>
       </c>
@@ -6010,7 +6230,7 @@
       </c>
       <c r="P72" s="45"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="31" t="s">
         <v>41</v>
       </c>
@@ -6052,7 +6272,7 @@
       </c>
       <c r="P73" s="45"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="31" t="s">
         <v>41</v>
       </c>
@@ -6098,7 +6318,7 @@
       </c>
       <c r="P74" s="45"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>41</v>
       </c>
@@ -6146,7 +6366,7 @@
       </c>
       <c r="P75" s="45"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="31" t="s">
         <v>41</v>
       </c>
@@ -6194,7 +6414,7 @@
       </c>
       <c r="P76" s="45"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="31" t="s">
         <v>41</v>
       </c>
@@ -6242,7 +6462,7 @@
       </c>
       <c r="P77" s="45"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="31" t="s">
         <v>41</v>
       </c>
@@ -6290,7 +6510,7 @@
       </c>
       <c r="P78" s="45"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="31" t="s">
         <v>41</v>
       </c>
@@ -6334,7 +6554,7 @@
       </c>
       <c r="P79" s="45"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="31" t="s">
         <v>41</v>
       </c>
@@ -6382,7 +6602,7 @@
       </c>
       <c r="P80" s="45"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="31" t="s">
         <v>41</v>
       </c>
@@ -6430,7 +6650,7 @@
       </c>
       <c r="P81" s="45"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="31" t="s">
         <v>41</v>
       </c>
@@ -6478,7 +6698,7 @@
       </c>
       <c r="P82" s="45"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="31" t="s">
         <v>41</v>
       </c>
@@ -6526,7 +6746,7 @@
       </c>
       <c r="P83" s="45"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="31" t="s">
         <v>41</v>
       </c>
@@ -6574,7 +6794,7 @@
       </c>
       <c r="P84" s="45"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="31" t="s">
         <v>41</v>
       </c>
@@ -6622,7 +6842,7 @@
       </c>
       <c r="P85" s="45"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="31" t="s">
         <v>41</v>
       </c>
@@ -6670,7 +6890,7 @@
       </c>
       <c r="P86" s="45"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>41</v>
       </c>
@@ -6716,7 +6936,7 @@
       </c>
       <c r="P87" s="45"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>41</v>
       </c>
@@ -6764,7 +6984,7 @@
       </c>
       <c r="P88" s="45"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="31" t="s">
         <v>41</v>
       </c>
@@ -6810,7 +7030,7 @@
       </c>
       <c r="P89" s="45"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="31" t="s">
         <v>41</v>
       </c>
@@ -6858,7 +7078,7 @@
       </c>
       <c r="P90" s="45"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="31" t="s">
         <v>41</v>
       </c>
@@ -6906,7 +7126,7 @@
       </c>
       <c r="P91" s="45"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
         <v>41</v>
       </c>
@@ -6954,7 +7174,7 @@
       </c>
       <c r="P92" s="45"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>41</v>
       </c>
@@ -7002,7 +7222,7 @@
       </c>
       <c r="P93" s="45"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="31" t="s">
         <v>41</v>
       </c>
@@ -7050,7 +7270,7 @@
       </c>
       <c r="P94" s="45"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="46" t="s">
         <v>41</v>
       </c>
@@ -7096,7 +7316,7 @@
       </c>
       <c r="P95" s="47"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="31" t="s">
         <v>36</v>
       </c>
@@ -7136,7 +7356,7 @@
       <c r="O96" s="31"/>
       <c r="P96" s="45"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="31" t="s">
         <v>16</v>
       </c>
@@ -7176,7 +7396,7 @@
       <c r="O97" s="31"/>
       <c r="P97" s="45"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="31" t="s">
         <v>185</v>
       </c>
@@ -7216,7 +7436,7 @@
       <c r="O98" s="31"/>
       <c r="P98" s="45"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="31" t="s">
         <v>185</v>
       </c>
@@ -7254,7 +7474,7 @@
       <c r="O99" s="31"/>
       <c r="P99" s="45"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="31" t="s">
         <v>189</v>
       </c>
@@ -7294,7 +7514,7 @@
       <c r="O100" s="31"/>
       <c r="P100" s="45"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="31" t="s">
         <v>192</v>
       </c>
@@ -7334,7 +7554,7 @@
       <c r="O101" s="31"/>
       <c r="P101" s="45"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="31" t="s">
         <v>189</v>
       </c>
@@ -7374,7 +7594,7 @@
       <c r="O102" s="31"/>
       <c r="P102" s="45"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" s="31" t="s">
         <v>189</v>
       </c>
@@ -7414,7 +7634,7 @@
       <c r="O103" s="31"/>
       <c r="P103" s="45"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" s="31" t="s">
         <v>89</v>
       </c>
@@ -7454,7 +7674,7 @@
       <c r="O104" s="31"/>
       <c r="P104" s="45"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" s="31" t="s">
         <v>198</v>
       </c>
@@ -7494,7 +7714,7 @@
       <c r="O105" s="31"/>
       <c r="P105" s="45"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="31" t="s">
         <v>41</v>
       </c>
@@ -7534,7 +7754,7 @@
       <c r="O106" s="31"/>
       <c r="P106" s="45"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="31" t="s">
         <v>41</v>
       </c>
@@ -7574,7 +7794,7 @@
       <c r="O107" s="31"/>
       <c r="P107" s="45"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="31" t="s">
         <v>41</v>
       </c>
@@ -7614,7 +7834,7 @@
       <c r="O108" s="31"/>
       <c r="P108" s="45"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="31" t="s">
         <v>204</v>
       </c>
@@ -7654,7 +7874,7 @@
       <c r="O109" s="31"/>
       <c r="P109" s="45"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" s="31" t="s">
         <v>41</v>
       </c>
@@ -7694,7 +7914,7 @@
       <c r="O110" s="31"/>
       <c r="P110" s="45"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" s="31" t="s">
         <v>73</v>
       </c>
@@ -7734,7 +7954,7 @@
       <c r="O111" s="31"/>
       <c r="P111" s="45"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" s="31" t="s">
         <v>41</v>
       </c>
@@ -7774,7 +7994,7 @@
       <c r="O112" s="31"/>
       <c r="P112" s="45"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" s="31" t="s">
         <v>68</v>
       </c>
@@ -7814,7 +8034,7 @@
       <c r="O113" s="31"/>
       <c r="P113" s="45"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" s="31" t="s">
         <v>68</v>
       </c>
@@ -7854,7 +8074,7 @@
       <c r="O114" s="31"/>
       <c r="P114" s="45"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" s="31" t="s">
         <v>68</v>
       </c>
@@ -7894,7 +8114,7 @@
       <c r="O115" s="31"/>
       <c r="P115" s="45"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" s="31" t="s">
         <v>216</v>
       </c>
@@ -7934,7 +8154,7 @@
       <c r="O116" s="31"/>
       <c r="P116" s="45"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" s="31" t="s">
         <v>216</v>
       </c>
@@ -7974,7 +8194,7 @@
       <c r="O117" s="31"/>
       <c r="P117" s="45"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" s="31" t="s">
         <v>216</v>
       </c>
@@ -8014,7 +8234,7 @@
       <c r="O118" s="31"/>
       <c r="P118" s="45"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" s="46" t="s">
         <v>221</v>
       </c>
@@ -8054,7 +8274,7 @@
       <c r="O119" s="46"/>
       <c r="P119" s="47"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" s="31" t="s">
         <v>221</v>
       </c>
@@ -8094,7 +8314,7 @@
       <c r="O120" s="31"/>
       <c r="P120" s="45"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" s="31" t="s">
         <v>225</v>
       </c>
@@ -8134,7 +8354,7 @@
       <c r="O121" s="31"/>
       <c r="P121" s="45"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" s="31" t="s">
         <v>228</v>
       </c>
@@ -8174,7 +8394,7 @@
       <c r="O122" s="31"/>
       <c r="P122" s="45"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" s="31" t="s">
         <v>228</v>
       </c>
@@ -8214,7 +8434,7 @@
       <c r="O123" s="31"/>
       <c r="P123" s="45"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" s="31" t="s">
         <v>101</v>
       </c>
@@ -8254,7 +8474,7 @@
       <c r="O124" s="31"/>
       <c r="P124" s="45"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" s="31" t="s">
         <v>101</v>
       </c>
@@ -8294,7 +8514,7 @@
       <c r="O125" s="31"/>
       <c r="P125" s="45"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" s="31" t="s">
         <v>101</v>
       </c>
@@ -8334,7 +8554,7 @@
       <c r="O126" s="31"/>
       <c r="P126" s="45"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" s="31" t="s">
         <v>93</v>
       </c>
@@ -8374,7 +8594,7 @@
       <c r="O127" s="31"/>
       <c r="P127" s="45"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" s="31" t="s">
         <v>236</v>
       </c>
@@ -8414,7 +8634,7 @@
       <c r="O128" s="31"/>
       <c r="P128" s="45"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" s="31" t="s">
         <v>239</v>
       </c>
@@ -8454,7 +8674,7 @@
       <c r="O129" s="31"/>
       <c r="P129" s="45"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" s="31" t="s">
         <v>41</v>
       </c>
@@ -8494,7 +8714,7 @@
       <c r="O130" s="31"/>
       <c r="P130" s="45"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" s="31" t="s">
         <v>41</v>
       </c>
@@ -8534,7 +8754,7 @@
       <c r="O131" s="31"/>
       <c r="P131" s="45"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" s="31" t="s">
         <v>41</v>
       </c>
@@ -8574,7 +8794,7 @@
       <c r="O132" s="31"/>
       <c r="P132" s="45"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" s="31" t="s">
         <v>41</v>
       </c>
@@ -8614,7 +8834,7 @@
       <c r="O133" s="31"/>
       <c r="P133" s="45"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" s="31" t="s">
         <v>41</v>
       </c>
@@ -8654,7 +8874,7 @@
       <c r="O134" s="31"/>
       <c r="P134" s="45"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" s="31" t="s">
         <v>41</v>
       </c>
@@ -8694,7 +8914,7 @@
       <c r="O135" s="31"/>
       <c r="P135" s="45"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" s="31" t="s">
         <v>41</v>
       </c>
@@ -8734,7 +8954,7 @@
       <c r="O136" s="31"/>
       <c r="P136" s="45"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" s="31" t="s">
         <v>41</v>
       </c>
@@ -8774,7 +8994,7 @@
       <c r="O137" s="31"/>
       <c r="P137" s="45"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" s="31" t="s">
         <v>41</v>
       </c>
@@ -8814,7 +9034,7 @@
       <c r="O138" s="31"/>
       <c r="P138" s="45"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" s="31" t="s">
         <v>41</v>
       </c>
@@ -8854,7 +9074,7 @@
       <c r="O139" s="31"/>
       <c r="P139" s="45"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" s="31" t="s">
         <v>41</v>
       </c>
@@ -8894,7 +9114,7 @@
       <c r="O140" s="31"/>
       <c r="P140" s="45"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" s="31" t="s">
         <v>41</v>
       </c>
@@ -8934,7 +9154,7 @@
       <c r="O141" s="31"/>
       <c r="P141" s="45"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" s="31" t="s">
         <v>41</v>
       </c>
@@ -8974,7 +9194,7 @@
       <c r="O142" s="31"/>
       <c r="P142" s="45"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" s="31" t="s">
         <v>68</v>
       </c>
@@ -9014,7 +9234,7 @@
       <c r="O143" s="31"/>
       <c r="P143" s="45"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" s="31" t="s">
         <v>68</v>
       </c>
@@ -9054,7 +9274,7 @@
       <c r="O144" s="31"/>
       <c r="P144" s="45"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" s="31" t="s">
         <v>68</v>
       </c>
@@ -9094,7 +9314,7 @@
       <c r="O145" s="31"/>
       <c r="P145" s="45"/>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" s="31" t="s">
         <v>68</v>
       </c>
@@ -9134,7 +9354,7 @@
       <c r="O146" s="46"/>
       <c r="P146" s="47"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" s="31"/>
       <c r="B147" s="31" t="s">
         <v>17</v>
@@ -9168,7 +9388,7 @@
       <c r="O147" s="31"/>
       <c r="P147" s="47"/>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" s="31"/>
       <c r="B148" s="31" t="s">
         <v>17</v>
@@ -9202,7 +9422,7 @@
       <c r="O148" s="31"/>
       <c r="P148" s="47"/>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" s="31"/>
       <c r="B149" s="31" t="s">
         <v>17</v>
@@ -9236,7 +9456,7 @@
       <c r="O149" s="31"/>
       <c r="P149" s="47"/>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" s="31"/>
       <c r="B150" s="31" t="s">
         <v>17</v>
@@ -9270,7 +9490,7 @@
       <c r="O150" s="31"/>
       <c r="P150" s="47"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" s="31"/>
       <c r="B151" s="31" t="s">
         <v>17</v>
@@ -9304,7 +9524,7 @@
       <c r="O151" s="31"/>
       <c r="P151" s="47"/>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" s="31" t="s">
         <v>97</v>
       </c>
@@ -9317,10 +9537,10 @@
       <c r="D152" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E152" s="31" t="s">
-        <v>288</v>
-      </c>
-      <c r="F152" s="31"/>
+      <c r="E152" s="53" t="s">
+        <v>310</v>
+      </c>
+      <c r="F152" s="53"/>
       <c r="G152" s="31" t="s">
         <v>22</v>
       </c>
@@ -9337,63 +9557,930 @@
         <v>100</v>
       </c>
       <c r="L152" s="29"/>
-      <c r="M152" s="31"/>
-      <c r="N152" s="31"/>
-      <c r="O152" s="31"/>
-      <c r="P152" s="47"/>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A153" s="31"/>
-      <c r="B153" s="31"/>
-      <c r="C153" s="31"/>
-      <c r="D153" s="31"/>
-      <c r="E153" s="31"/>
-      <c r="F153" s="31"/>
-      <c r="G153" s="31"/>
-      <c r="H153" s="31"/>
-      <c r="I153" s="31"/>
-      <c r="J153" s="31"/>
-      <c r="K153" s="31"/>
-      <c r="M153" s="31"/>
-      <c r="N153" s="31"/>
-      <c r="O153" s="31"/>
-      <c r="P153" s="47"/>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A154" s="31"/>
-      <c r="B154" s="31"/>
-      <c r="C154" s="31"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="31"/>
-      <c r="G154" s="31"/>
-      <c r="H154" s="31"/>
-      <c r="I154" s="31"/>
-      <c r="J154" s="31"/>
-      <c r="K154" s="31"/>
-      <c r="M154" s="31"/>
-      <c r="N154" s="31"/>
-      <c r="O154" s="31"/>
-      <c r="P154" s="47"/>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A155" s="31"/>
-      <c r="B155" s="31"/>
-      <c r="C155" s="31"/>
-      <c r="D155" s="31"/>
-      <c r="E155" s="31"/>
-      <c r="F155" s="31"/>
-      <c r="G155" s="31"/>
-      <c r="H155" s="31"/>
-      <c r="I155" s="31"/>
-      <c r="J155" s="31"/>
-      <c r="K155" s="31"/>
-      <c r="M155" s="31"/>
-      <c r="N155" s="31"/>
-      <c r="O155" s="31"/>
-      <c r="P155" s="47"/>
+      <c r="M152" s="53"/>
+      <c r="N152" s="53"/>
+      <c r="O152" s="53"/>
+      <c r="P152" s="54"/>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A153" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B153" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C153" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D153" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E153" s="53" t="s">
+        <v>311</v>
+      </c>
+      <c r="F153" s="53"/>
+      <c r="G153" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H153" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I153" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J153" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K153" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L153" s="29"/>
+      <c r="M153" s="53"/>
+      <c r="N153" s="53"/>
+      <c r="O153" s="53"/>
+      <c r="P153" s="54"/>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A154" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B154" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C154" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D154" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E154" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="F154" s="53"/>
+      <c r="G154" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H154" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I154" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J154" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K154" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L154" s="29"/>
+      <c r="M154" s="53"/>
+      <c r="N154" s="53"/>
+      <c r="O154" s="53"/>
+      <c r="P154" s="54"/>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A155" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B155" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D155" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E155" s="53" t="s">
+        <v>313</v>
+      </c>
+      <c r="F155" s="53"/>
+      <c r="G155" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H155" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I155" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J155" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K155" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L155" s="29"/>
+      <c r="M155" s="53"/>
+      <c r="N155" s="53"/>
+      <c r="O155" s="53"/>
+      <c r="P155" s="54"/>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A156" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B156" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C156" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D156" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E156" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="F156" s="31"/>
+      <c r="G156" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H156" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I156" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J156" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K156" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L156" s="29"/>
+      <c r="M156" s="31"/>
+      <c r="N156" s="31"/>
+      <c r="O156" s="31"/>
+      <c r="P156" s="47"/>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A157" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B157" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C157" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E157" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="F157" s="31"/>
+      <c r="G157" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H157" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I157" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J157" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K157" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L157" s="29"/>
+      <c r="M157" s="31"/>
+      <c r="N157" s="31"/>
+      <c r="O157" s="31"/>
+      <c r="P157" s="47"/>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A158" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B158" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C158" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D158" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E158" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="F158" s="31"/>
+      <c r="G158" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H158" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I158" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J158" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K158" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L158" s="29"/>
+      <c r="M158" s="31"/>
+      <c r="N158" s="31"/>
+      <c r="O158" s="31"/>
+      <c r="P158" s="47"/>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A159" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B159" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C159" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D159" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E159" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="F159" s="31"/>
+      <c r="G159" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H159" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I159" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J159" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K159" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L159" s="29"/>
+      <c r="M159" s="31"/>
+      <c r="N159" s="31"/>
+      <c r="O159" s="31"/>
+      <c r="P159" s="47"/>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A160" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B160" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D160" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E160" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="F160" s="46"/>
+      <c r="G160" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H160" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I160" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J160" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K160" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L160" s="52"/>
+      <c r="M160" s="46"/>
+      <c r="N160" s="46"/>
+      <c r="O160" s="46"/>
+      <c r="P160" s="47"/>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A161" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B161" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C161" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D161" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E161" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="F161" s="46"/>
+      <c r="G161" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H161" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I161" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J161" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K161" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L161" s="52"/>
+      <c r="M161" s="46"/>
+      <c r="N161" s="46"/>
+      <c r="O161" s="46"/>
+      <c r="P161" s="47"/>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A162" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B162" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C162" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D162" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E162" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H162" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I162" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J162" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K162" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L162" s="52"/>
+      <c r="M162" s="46"/>
+      <c r="N162" s="46"/>
+      <c r="O162" s="46"/>
+      <c r="P162" s="47"/>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A163" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B163" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C163" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D163" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E163" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="F163" s="46"/>
+      <c r="G163" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H163" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I163" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J163" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K163" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L163" s="52"/>
+      <c r="M163" s="46"/>
+      <c r="N163" s="46"/>
+      <c r="O163" s="46"/>
+      <c r="P163" s="47"/>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A164" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B164" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C164" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D164" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E164" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="F164" s="46"/>
+      <c r="G164" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H164" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I164" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J164" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K164" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L164" s="52"/>
+      <c r="M164" s="46"/>
+      <c r="N164" s="46"/>
+      <c r="O164" s="46"/>
+      <c r="P164" s="47"/>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A165" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B165" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C165" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D165" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E165" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="F165" s="46"/>
+      <c r="G165" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H165" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I165" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J165" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K165" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L165" s="52"/>
+      <c r="M165" s="46"/>
+      <c r="N165" s="46"/>
+      <c r="O165" s="46"/>
+      <c r="P165" s="47"/>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A166" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B166" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C166" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D166" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E166" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="F166" s="46"/>
+      <c r="G166" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H166" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I166" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J166" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K166" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L166" s="52"/>
+      <c r="M166" s="46"/>
+      <c r="N166" s="46"/>
+      <c r="O166" s="46"/>
+      <c r="P166" s="47"/>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A167" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B167" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C167" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D167" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E167" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="F167" s="46"/>
+      <c r="G167" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H167" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I167" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J167" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K167" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L167" s="52"/>
+      <c r="M167" s="46"/>
+      <c r="N167" s="46"/>
+      <c r="O167" s="46"/>
+      <c r="P167" s="47"/>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A168" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B168" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C168" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D168" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E168" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="F168" s="46"/>
+      <c r="G168" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H168" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I168" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J168" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K168" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L168" s="52"/>
+      <c r="M168" s="46"/>
+      <c r="N168" s="46"/>
+      <c r="O168" s="46"/>
+      <c r="P168" s="47"/>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A169" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B169" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C169" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D169" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E169" s="46" t="s">
+        <v>300</v>
+      </c>
+      <c r="F169" s="46"/>
+      <c r="G169" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H169" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I169" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J169" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K169" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L169" s="52"/>
+      <c r="M169" s="46"/>
+      <c r="N169" s="46"/>
+      <c r="O169" s="46"/>
+      <c r="P169" s="47"/>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A170" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B170" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C170" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D170" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E170" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="F170" s="55"/>
+      <c r="G170" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H170" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I170" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J170" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K170" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L170" s="52"/>
+      <c r="M170" s="55"/>
+      <c r="N170" s="55"/>
+      <c r="O170" s="55"/>
+      <c r="P170" s="56"/>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A171" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B171" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C171" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D171" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E171" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="F171" s="55"/>
+      <c r="G171" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H171" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I171" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J171" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K171" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L171" s="52"/>
+      <c r="M171" s="55"/>
+      <c r="N171" s="55"/>
+      <c r="O171" s="55"/>
+      <c r="P171" s="56"/>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A172" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B172" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C172" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D172" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E172" s="55" t="s">
+        <v>304</v>
+      </c>
+      <c r="F172" s="55"/>
+      <c r="G172" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H172" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I172" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J172" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K172" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L172" s="52"/>
+      <c r="M172" s="55"/>
+      <c r="N172" s="55"/>
+      <c r="O172" s="55"/>
+      <c r="P172" s="56"/>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A173" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B173" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C173" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D173" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E173" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="F173" s="55"/>
+      <c r="G173" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H173" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I173" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J173" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K173" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L173" s="52"/>
+      <c r="M173" s="55"/>
+      <c r="N173" s="55"/>
+      <c r="O173" s="55"/>
+      <c r="P173" s="56"/>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A174" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B174" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C174" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D174" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E174" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="F174" s="55"/>
+      <c r="G174" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H174" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I174" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J174" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K174" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L174" s="52"/>
+      <c r="M174" s="55"/>
+      <c r="N174" s="55"/>
+      <c r="O174" s="55"/>
+      <c r="P174" s="56"/>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A175" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B175" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C175" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D175" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E175" s="55" t="s">
+        <v>307</v>
+      </c>
+      <c r="F175" s="55"/>
+      <c r="G175" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H175" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I175" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J175" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K175" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L175" s="52"/>
+      <c r="M175" s="55"/>
+      <c r="N175" s="55"/>
+      <c r="O175" s="55"/>
+      <c r="P175" s="56"/>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A176" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B176" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C176" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D176" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E176" s="55" t="s">
+        <v>308</v>
+      </c>
+      <c r="F176" s="55"/>
+      <c r="G176" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H176" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I176" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J176" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K176" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L176" s="52"/>
+      <c r="M176" s="55"/>
+      <c r="N176" s="55"/>
+      <c r="O176" s="55"/>
+      <c r="P176" s="56"/>
+    </row>
+    <row r="181" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K181" t="s">
+        <v>309</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B16">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"X,X,X"</formula>
@@ -9404,7 +10491,7 @@
       <formula>"X,X,X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:J1048576 B39 B110:B134">
+  <conditionalFormatting sqref="B39 B110:B134 G1:J1048576">
     <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"X,X,X"</formula>
     </cfRule>
@@ -9426,7 +10513,7 @@
       <formula>"Doorgevoerd"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L155">
+  <conditionalFormatting sqref="L2:L176">
     <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"In pull request"</formula>
     </cfRule>
@@ -9445,13 +10532,13 @@
           <x14:formula1>
             <xm:f>Configuratie!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L1 L116:L134 L96:L98 L100:L114 L153:L1048576</xm:sqref>
+          <xm:sqref>L1 L116:L134 L96:L98 L100:L114 L177:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A99B45A-3469-41B9-95C3-9470E9A47E8F}">
           <x14:formula1>
             <xm:f>Configuratie!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L135:L152 L99 L115 L2:L95</xm:sqref>
+          <xm:sqref>L135:L176 L99 L115 L2:L95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2067B2B-AAB7-4BB4-AB95-6ECCB20F9551}">
           <x14:formula1>
@@ -9485,23 +10572,23 @@
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -9542,7 +10629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -9557,7 +10644,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="20"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -9572,7 +10659,7 @@
       <c r="L3" s="16"/>
       <c r="M3" s="20"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -9587,7 +10674,7 @@
       <c r="L4" s="16"/>
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -9602,7 +10689,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -9617,7 +10704,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -9632,7 +10719,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -9647,7 +10734,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -9662,7 +10749,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -9677,7 +10764,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -9693,7 +10780,7 @@
       <c r="M11" s="22"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -9709,7 +10796,7 @@
       <c r="M12" s="22"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -9725,7 +10812,7 @@
       <c r="M13" s="22"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -9741,7 +10828,7 @@
       <c r="M14" s="22"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -9757,7 +10844,7 @@
       <c r="M15" s="21"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -9773,7 +10860,7 @@
       <c r="M16" s="21"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -9789,7 +10876,7 @@
       <c r="M17" s="21"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -9804,7 +10891,7 @@
       <c r="L18" s="16"/>
       <c r="M18" s="20"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -9819,7 +10906,7 @@
       <c r="L19" s="16"/>
       <c r="M19" s="20"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -9834,7 +10921,7 @@
       <c r="L20" s="16"/>
       <c r="M20" s="20"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -9849,7 +10936,7 @@
       <c r="L21" s="16"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -9864,7 +10951,7 @@
       <c r="L22" s="16"/>
       <c r="M22" s="20"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -9879,7 +10966,7 @@
       <c r="L23" s="16"/>
       <c r="M23" s="20"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -9894,7 +10981,7 @@
       <c r="L24" s="16"/>
       <c r="M24" s="20"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -9998,16 +11085,16 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>266</v>
       </c>
@@ -10024,7 +11111,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>6</v>
       </c>
@@ -10041,7 +11128,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>27</v>
       </c>
@@ -10058,7 +11145,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>26</v>
       </c>
@@ -10075,7 +11162,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>25</v>
       </c>
@@ -10092,7 +11179,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>24</v>
       </c>
@@ -10109,7 +11196,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>23</v>
       </c>
@@ -10126,7 +11213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -10143,7 +11230,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>4</v>
       </c>
@@ -10160,7 +11247,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>3</v>
       </c>
@@ -10177,7 +11264,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -10194,7 +11281,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>28</v>
       </c>
@@ -10211,7 +11298,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>21</v>
       </c>
@@ -10228,7 +11315,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>20</v>
       </c>
@@ -10245,7 +11332,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>19</v>
       </c>
@@ -10262,7 +11349,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>18</v>
       </c>
@@ -10279,7 +11366,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>17</v>
       </c>
@@ -10296,7 +11383,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -10313,7 +11400,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -10330,7 +11417,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -10347,7 +11434,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>13</v>
       </c>
@@ -10364,7 +11451,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -10381,7 +11468,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>12</v>
       </c>
@@ -10398,7 +11485,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>11</v>
       </c>
@@ -10415,7 +11502,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>10</v>
       </c>
@@ -10432,7 +11519,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>9</v>
       </c>
@@ -10449,7 +11536,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>8</v>
       </c>
@@ -10466,7 +11553,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>7</v>
       </c>
@@ -10483,7 +11570,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>22</v>
       </c>
@@ -10514,42 +11601,42 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>287</v>
       </c>
@@ -10560,26 +11647,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="030eaba2-629b-4e56-920e-8dcc1358a952">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100515BA15BA15D264586723D52FB60ADE3" ma:contentTypeVersion="16" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f61f07c867748b0019541a657f349ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xmlns:ns3="030eaba2-629b-4e56-920e-8dcc1358a952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5688d83df968b8ed30cda1c17f9d8ac7" ns2:_="" ns3:_="">
     <xsd:import namespace="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
@@ -10820,26 +11887,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B0455E-EE44-411A-9909-1872C21A7AE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D83BA7-0BB7-4894-A3C1-EDDBDFCC6BB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="030eaba2-629b-4e56-920e-8dcc1358a952"/>
-    <ds:schemaRef ds:uri="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="030eaba2-629b-4e56-920e-8dcc1358a952">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FF6D437-CC37-4CBE-9DFE-67A70FDDA4C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10858,6 +11926,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B0455E-EE44-411A-9909-1872C21A7AE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D83BA7-0BB7-4894-A3C1-EDDBDFCC6BB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="030eaba2-629b-4e56-920e-8dcc1358a952"/>
+    <ds:schemaRef ds:uri="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e36377b7-70c4-4493-a338-095918d327e9}" enabled="0" method="" siteId="{e36377b7-70c4-4493-a338-095918d327e9}" removed="1"/>

</xml_diff>

<commit_message>
SSDLC voorzien van TC1
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eb0095856\Projecten\Leerlijn-Content-SE-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DDF457-4D4B-4536-83CC-D00885F13F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8084C7B4-E109-480B-A045-CF7AF8B696A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{7013DF88-B919-4E44-A3B6-EFF7F9C231E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7013DF88-B919-4E44-A3B6-EFF7F9C231E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="314">
   <si>
     <t>TC-1</t>
   </si>
@@ -1441,7 +1441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1499,15 +1499,11 @@
     <xf numFmtId="0" fontId="9" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="62">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1705,146 +1701,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2886,61 +2742,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}" name="Tabel3" displayName="Tabel3" ref="A1:P176" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}" name="Tabel3" displayName="Tabel3" ref="A1:P176" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58">
   <autoFilter ref="A1:P176" xr:uid="{98B2741E-2F52-40E8-B271-0C73FC0EFEB8}"/>
   <tableColumns count="16">
-    <tableColumn id="2" xr3:uid="{F8A50546-3BB2-41F8-99A7-821FFAEA9EA0}" name="TC-1" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{41734F87-6DB1-4AC3-80CE-250B23378554}" name="TC-2" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{5B30DF97-0362-47CA-9FEB-983BDA2DF844}" name="Proces" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{DDC7FBE8-1A18-4596-8FBD-1F40B9F94AA0}" name="Processtap" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{15170496-2005-43A7-AD43-CFD4F0B25656}" name="Onderwerp" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{AD473AEC-8FAD-46C0-A48A-A65E296DBE11}" name="PS" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{1591AA9A-3ED6-44E5-A48A-E9910C5A2DDC}" name="LT" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{343866B0-4820-4E45-9596-524C0A3E0DB4}" name="OI" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{B3D04D72-920A-4859-8170-8854154E6BEE}" name="PI" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{DAE26EF7-02E2-4493-9827-F044C9947102}" name="DT" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{66861921-DC42-4E48-9995-22D71902D0E6}" name="Auteur" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{F8A50546-3BB2-41F8-99A7-821FFAEA9EA0}" name="TC-1" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{41734F87-6DB1-4AC3-80CE-250B23378554}" name="TC-2" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{5B30DF97-0362-47CA-9FEB-983BDA2DF844}" name="Proces" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{DDC7FBE8-1A18-4596-8FBD-1F40B9F94AA0}" name="Processtap" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{15170496-2005-43A7-AD43-CFD4F0B25656}" name="Onderwerp" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{AD473AEC-8FAD-46C0-A48A-A65E296DBE11}" name="PS" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{1591AA9A-3ED6-44E5-A48A-E9910C5A2DDC}" name="LT" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{343866B0-4820-4E45-9596-524C0A3E0DB4}" name="OI" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{B3D04D72-920A-4859-8170-8854154E6BEE}" name="PI" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{DAE26EF7-02E2-4493-9827-F044C9947102}" name="DT" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{66861921-DC42-4E48-9995-22D71902D0E6}" name="Auteur" dataDxfId="47"/>
     <tableColumn id="13" xr3:uid="{41E829DC-30B4-4ED6-A23E-6E86A90CC847}" name="Status"/>
-    <tableColumn id="14" xr3:uid="{4DEA7C20-4CDB-4765-A2ED-2DAE0C74EA88}" name="Les" dataDxfId="60"/>
-    <tableColumn id="15" xr3:uid="{BA1A1DC9-E1C8-41C8-8B22-98655139BA61}" name="Week" dataDxfId="59"/>
-    <tableColumn id="16" xr3:uid="{FEFBF060-7975-4841-BB25-4FD9EA20FCE9}" name="Vak" dataDxfId="58"/>
-    <tableColumn id="17" xr3:uid="{DC49865F-5E2A-4A41-9018-4460A5231335}" name="Opmerking" dataDxfId="57"/>
+    <tableColumn id="14" xr3:uid="{4DEA7C20-4CDB-4765-A2ED-2DAE0C74EA88}" name="Les" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{BA1A1DC9-E1C8-41C8-8B22-98655139BA61}" name="Week" dataDxfId="45"/>
+    <tableColumn id="16" xr3:uid="{FEFBF060-7975-4841-BB25-4FD9EA20FCE9}" name="Vak" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{DC49865F-5E2A-4A41-9018-4460A5231335}" name="Opmerking" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}" name="Tabel46" displayName="Tabel46" ref="A1:M25" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}" name="Tabel46" displayName="Tabel46" ref="A1:M25" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:M25" xr:uid="{6339E1F4-F4B6-4657-9A4C-D6B1F30A8DA6}"/>
   <tableColumns count="13">
-    <tableColumn id="2" xr3:uid="{1535D98C-E0EE-4D42-BCEB-E5B9CE3EB61D}" name="TC-1" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{626D3CCE-98FA-446A-9492-EFF5B77FBEE7}" name="TC-2" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{7D9467F0-D231-479A-AC4D-EFCFCDA0F355}" name="Proces" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{563F1A23-B95F-4820-8982-FD4C397E7132}" name="Processtap" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{6EB4EFB7-2E6E-49E8-8B36-E5A953066F34}" name="Onderwerp" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{952C00F6-C03B-46BB-8BDD-48716B660A03}" name="PS" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{905E3EDF-F38D-471C-BAF6-5E4C96FF3FB2}" name="LT" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{8DFE5EC7-2595-4617-8FC0-FDDA89438F44}" name="OI" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{557B5D16-5B65-4AF7-BD7B-FB0218A7C1B3}" name="PI" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{9F6BDCD6-BD58-4752-B392-4BDB07F65BF9}" name="DT" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{265C90D0-C2F9-46F3-BC15-46853C80AE44}" name="Auteur" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{56238B06-B929-4176-9193-3DBF61BD24F4}" name="Reviewer" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{5A7CC1D3-6CDF-46C8-BAD6-5021F68425FC}" name="Status" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{1535D98C-E0EE-4D42-BCEB-E5B9CE3EB61D}" name="TC-1" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{626D3CCE-98FA-446A-9492-EFF5B77FBEE7}" name="TC-2" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{7D9467F0-D231-479A-AC4D-EFCFCDA0F355}" name="Proces" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{563F1A23-B95F-4820-8982-FD4C397E7132}" name="Processtap" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{6EB4EFB7-2E6E-49E8-8B36-E5A953066F34}" name="Onderwerp" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{952C00F6-C03B-46BB-8BDD-48716B660A03}" name="PS" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{905E3EDF-F38D-471C-BAF6-5E4C96FF3FB2}" name="LT" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{8DFE5EC7-2595-4617-8FC0-FDDA89438F44}" name="OI" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{557B5D16-5B65-4AF7-BD7B-FB0218A7C1B3}" name="PI" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{9F6BDCD6-BD58-4752-B392-4BDB07F65BF9}" name="DT" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{265C90D0-C2F9-46F3-BC15-46853C80AE44}" name="Auteur" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{56238B06-B929-4176-9193-3DBF61BD24F4}" name="Reviewer" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{5A7CC1D3-6CDF-46C8-BAD6-5021F68425FC}" name="Status" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}" name="Tabel2" displayName="Tabel2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}" name="Tabel2" displayName="Tabel2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:E29" xr:uid="{2A682B7F-49AE-4DC6-9468-B67CCC93E610}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E0D87A47-D7F7-498A-A22E-05A996992FE5}" name="Id" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{A3888C5B-B532-4621-A573-477CB568DA88}" name="SSDLC" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E1227983-22D3-4B85-9382-7BE0428CF806}" name="Proces" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{25EAD8F8-D89A-4F34-8AE3-23D6D7363D47}" name="Processtap" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{DCD8D2DD-F7D1-48E7-8B06-F484930BAD1C}" name="Taxonomiecode-deel-1" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{E0D87A47-D7F7-498A-A22E-05A996992FE5}" name="Id" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{A3888C5B-B532-4621-A573-477CB568DA88}" name="SSDLC" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{E1227983-22D3-4B85-9382-7BE0428CF806}" name="Proces" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{25EAD8F8-D89A-4F34-8AE3-23D6D7363D47}" name="Processtap" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{DCD8D2DD-F7D1-48E7-8B06-F484930BAD1C}" name="Taxonomiecode-deel-1" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3265,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C8AE46-0301-40E0-97E1-E2E70FD5D32D}">
   <dimension ref="A1:P181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9355,11 +9211,15 @@
       <c r="P146" s="47"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A147" s="31"/>
+      <c r="A147" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B147" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C147" s="31"/>
+      <c r="C147" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="D147" s="31"/>
       <c r="E147" s="31" t="s">
         <v>259</v>
@@ -9389,11 +9249,15 @@
       <c r="P147" s="47"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A148" s="31"/>
+      <c r="A148" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B148" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C148" s="31"/>
+      <c r="C148" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="D148" s="31"/>
       <c r="E148" s="31" t="s">
         <v>261</v>
@@ -9423,11 +9287,15 @@
       <c r="P148" s="47"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A149" s="31"/>
+      <c r="A149" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B149" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C149" s="31"/>
+      <c r="C149" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="D149" s="31"/>
       <c r="E149" s="31" t="s">
         <v>262</v>
@@ -9457,11 +9325,15 @@
       <c r="P149" s="47"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A150" s="31"/>
+      <c r="A150" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B150" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C150" s="31"/>
+      <c r="C150" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="D150" s="31"/>
       <c r="E150" s="31" t="s">
         <v>263</v>
@@ -9491,11 +9363,15 @@
       <c r="P150" s="47"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A151" s="31"/>
+      <c r="A151" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B151" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C151" s="31"/>
+      <c r="C151" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="D151" s="31"/>
       <c r="E151" s="31" t="s">
         <v>264</v>
@@ -9537,10 +9413,10 @@
       <c r="D152" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E152" s="53" t="s">
+      <c r="E152" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="F152" s="53"/>
+      <c r="F152" s="31"/>
       <c r="G152" s="31" t="s">
         <v>22</v>
       </c>
@@ -9557,10 +9433,10 @@
         <v>100</v>
       </c>
       <c r="L152" s="29"/>
-      <c r="M152" s="53"/>
-      <c r="N152" s="53"/>
-      <c r="O152" s="53"/>
-      <c r="P152" s="54"/>
+      <c r="M152" s="31"/>
+      <c r="N152" s="31"/>
+      <c r="O152" s="31"/>
+      <c r="P152" s="45"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" s="31" t="s">
@@ -9575,10 +9451,10 @@
       <c r="D153" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E153" s="53" t="s">
+      <c r="E153" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="F153" s="53"/>
+      <c r="F153" s="31"/>
       <c r="G153" s="31" t="s">
         <v>22</v>
       </c>
@@ -9595,10 +9471,10 @@
         <v>100</v>
       </c>
       <c r="L153" s="29"/>
-      <c r="M153" s="53"/>
-      <c r="N153" s="53"/>
-      <c r="O153" s="53"/>
-      <c r="P153" s="54"/>
+      <c r="M153" s="31"/>
+      <c r="N153" s="31"/>
+      <c r="O153" s="31"/>
+      <c r="P153" s="45"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" s="31" t="s">
@@ -9613,10 +9489,10 @@
       <c r="D154" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E154" s="53" t="s">
+      <c r="E154" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="F154" s="53"/>
+      <c r="F154" s="31"/>
       <c r="G154" s="31" t="s">
         <v>22</v>
       </c>
@@ -9633,10 +9509,10 @@
         <v>100</v>
       </c>
       <c r="L154" s="29"/>
-      <c r="M154" s="53"/>
-      <c r="N154" s="53"/>
-      <c r="O154" s="53"/>
-      <c r="P154" s="54"/>
+      <c r="M154" s="31"/>
+      <c r="N154" s="31"/>
+      <c r="O154" s="31"/>
+      <c r="P154" s="45"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" s="31" t="s">
@@ -9651,10 +9527,10 @@
       <c r="D155" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E155" s="53" t="s">
+      <c r="E155" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="F155" s="53"/>
+      <c r="F155" s="31"/>
       <c r="G155" s="31" t="s">
         <v>22</v>
       </c>
@@ -9671,10 +9547,10 @@
         <v>100</v>
       </c>
       <c r="L155" s="29"/>
-      <c r="M155" s="53"/>
-      <c r="N155" s="53"/>
-      <c r="O155" s="53"/>
-      <c r="P155" s="54"/>
+      <c r="M155" s="31"/>
+      <c r="N155" s="31"/>
+      <c r="O155" s="31"/>
+      <c r="P155" s="45"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" s="31" t="s">
@@ -10221,10 +10097,10 @@
       <c r="D170" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E170" s="55" t="s">
+      <c r="E170" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="F170" s="55"/>
+      <c r="F170" s="46"/>
       <c r="G170" s="46" t="s">
         <v>22</v>
       </c>
@@ -10241,10 +10117,10 @@
         <v>100</v>
       </c>
       <c r="L170" s="52"/>
-      <c r="M170" s="55"/>
-      <c r="N170" s="55"/>
-      <c r="O170" s="55"/>
-      <c r="P170" s="56"/>
+      <c r="M170" s="46"/>
+      <c r="N170" s="46"/>
+      <c r="O170" s="46"/>
+      <c r="P170" s="47"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" s="46" t="s">
@@ -10259,10 +10135,10 @@
       <c r="D171" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E171" s="55" t="s">
+      <c r="E171" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F171" s="55"/>
+      <c r="F171" s="46"/>
       <c r="G171" s="46" t="s">
         <v>22</v>
       </c>
@@ -10279,10 +10155,10 @@
         <v>100</v>
       </c>
       <c r="L171" s="52"/>
-      <c r="M171" s="55"/>
-      <c r="N171" s="55"/>
-      <c r="O171" s="55"/>
-      <c r="P171" s="56"/>
+      <c r="M171" s="46"/>
+      <c r="N171" s="46"/>
+      <c r="O171" s="46"/>
+      <c r="P171" s="47"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" s="46" t="s">
@@ -10297,10 +10173,10 @@
       <c r="D172" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E172" s="55" t="s">
+      <c r="E172" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="F172" s="55"/>
+      <c r="F172" s="46"/>
       <c r="G172" s="46" t="s">
         <v>22</v>
       </c>
@@ -10317,10 +10193,10 @@
         <v>100</v>
       </c>
       <c r="L172" s="52"/>
-      <c r="M172" s="55"/>
-      <c r="N172" s="55"/>
-      <c r="O172" s="55"/>
-      <c r="P172" s="56"/>
+      <c r="M172" s="46"/>
+      <c r="N172" s="46"/>
+      <c r="O172" s="46"/>
+      <c r="P172" s="47"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" s="46" t="s">
@@ -10335,10 +10211,10 @@
       <c r="D173" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E173" s="55" t="s">
+      <c r="E173" s="46" t="s">
         <v>305</v>
       </c>
-      <c r="F173" s="55"/>
+      <c r="F173" s="46"/>
       <c r="G173" s="46" t="s">
         <v>22</v>
       </c>
@@ -10355,10 +10231,10 @@
         <v>100</v>
       </c>
       <c r="L173" s="52"/>
-      <c r="M173" s="55"/>
-      <c r="N173" s="55"/>
-      <c r="O173" s="55"/>
-      <c r="P173" s="56"/>
+      <c r="M173" s="46"/>
+      <c r="N173" s="46"/>
+      <c r="O173" s="46"/>
+      <c r="P173" s="47"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="46" t="s">
@@ -10373,10 +10249,10 @@
       <c r="D174" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E174" s="55" t="s">
+      <c r="E174" s="46" t="s">
         <v>306</v>
       </c>
-      <c r="F174" s="55"/>
+      <c r="F174" s="46"/>
       <c r="G174" s="46" t="s">
         <v>22</v>
       </c>
@@ -10393,10 +10269,10 @@
         <v>100</v>
       </c>
       <c r="L174" s="52"/>
-      <c r="M174" s="55"/>
-      <c r="N174" s="55"/>
-      <c r="O174" s="55"/>
-      <c r="P174" s="56"/>
+      <c r="M174" s="46"/>
+      <c r="N174" s="46"/>
+      <c r="O174" s="46"/>
+      <c r="P174" s="47"/>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" s="46" t="s">
@@ -10411,10 +10287,10 @@
       <c r="D175" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E175" s="55" t="s">
+      <c r="E175" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="F175" s="55"/>
+      <c r="F175" s="46"/>
       <c r="G175" s="46" t="s">
         <v>22</v>
       </c>
@@ -10431,10 +10307,10 @@
         <v>100</v>
       </c>
       <c r="L175" s="52"/>
-      <c r="M175" s="55"/>
-      <c r="N175" s="55"/>
-      <c r="O175" s="55"/>
-      <c r="P175" s="56"/>
+      <c r="M175" s="46"/>
+      <c r="N175" s="46"/>
+      <c r="O175" s="46"/>
+      <c r="P175" s="47"/>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" s="46" t="s">
@@ -10449,10 +10325,10 @@
       <c r="D176" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E176" s="55" t="s">
+      <c r="E176" s="46" t="s">
         <v>308</v>
       </c>
-      <c r="F176" s="55"/>
+      <c r="F176" s="46"/>
       <c r="G176" s="46" t="s">
         <v>22</v>
       </c>
@@ -10469,10 +10345,10 @@
         <v>100</v>
       </c>
       <c r="L176" s="52"/>
-      <c r="M176" s="55"/>
-      <c r="N176" s="55"/>
-      <c r="O176" s="55"/>
-      <c r="P176" s="56"/>
+      <c r="M176" s="46"/>
+      <c r="N176" s="46"/>
+      <c r="O176" s="46"/>
+      <c r="P176" s="47"/>
     </row>
     <row r="181" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K181" t="s">
@@ -10491,7 +10367,7 @@
       <formula>"X,X,X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39 B110:B134 G1:J1048576">
+  <conditionalFormatting sqref="G1:J1048576 B39 B110:B134">
     <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"X,X,X"</formula>
     </cfRule>
@@ -11647,6 +11523,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="030eaba2-629b-4e56-920e-8dcc1358a952">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100515BA15BA15D264586723D52FB60ADE3" ma:contentTypeVersion="16" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f61f07c867748b0019541a657f349ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xmlns:ns3="030eaba2-629b-4e56-920e-8dcc1358a952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5688d83df968b8ed30cda1c17f9d8ac7" ns2:_="" ns3:_="">
     <xsd:import namespace="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
@@ -11887,27 +11783,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D83BA7-0BB7-4894-A3C1-EDDBDFCC6BB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="030eaba2-629b-4e56-920e-8dcc1358a952"/>
+    <ds:schemaRef ds:uri="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="030eaba2-629b-4e56-920e-8dcc1358a952">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B0455E-EE44-411A-9909-1872C21A7AE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FF6D437-CC37-4CBE-9DFE-67A70FDDA4C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11926,25 +11821,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B0455E-EE44-411A-9909-1872C21A7AE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D83BA7-0BB7-4894-A3C1-EDDBDFCC6BB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="030eaba2-629b-4e56-920e-8dcc1358a952"/>
-    <ds:schemaRef ds:uri="bb274f1b-0e95-4afa-93a7-e92bcbf9a51a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e36377b7-70c4-4493-a338-095918d327e9}" enabled="0" method="" siteId="{e36377b7-70c4-4493-a338-095918d327e9}" removed="1"/>

</xml_diff>